<commit_message>
segunda actualizacion de datos
</commit_message>
<xml_diff>
--- a/datos/rend-datos.xlsx
+++ b/datos/rend-datos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walter\Documents\1-1-1-1-DASHBOARD-INTERESANTES-STREAMLIT-PYTHON\regresion-analisys-predicted\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walter\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16272" windowHeight="8508"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16644" windowHeight="6348"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -410,7 +410,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,18 +587,32 @@
         <v>5.2750675405256629E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>45639</v>
+        <v>45657</v>
       </c>
       <c r="B13" s="3">
-        <v>1.0373638638845207E-2</v>
+        <v>-4.0456817157672728E-2</v>
       </c>
       <c r="C13" s="3">
-        <v>7.6572860482623153E-3</v>
+        <v>0.11504492669835839</v>
       </c>
       <c r="D13" s="3">
-        <v>3.0945720306804884E-3</v>
+        <v>5.7729375378128042E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>45658</v>
+      </c>
+      <c r="B14" s="3">
+        <v>3.3412105974565356E-2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.43513334946172311</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.2149864263526432</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>